<commit_message>
this is my twentyseventh commit
</commit_message>
<xml_diff>
--- a/testData/TC_StorageGridConfig.xlsx
+++ b/testData/TC_StorageGridConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilr2\eclipse-workspace\UCPQ_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4A4469-B691-444D-BF2C-37801D343223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDB87F2-2B87-4D0C-8BA0-AABC39B2E5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Username</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Qty Storage Nodes</t>
   </si>
   <si>
-    <t>Test Second Automation</t>
-  </si>
-  <si>
     <t>Opportunity Name</t>
   </si>
   <si>
@@ -163,6 +160,24 @@
   </si>
   <si>
     <t>StorageGRID Appliance</t>
+  </si>
+  <si>
+    <t>Test-Automation-Indirect</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>Reseller through NetApp</t>
+  </si>
+  <si>
+    <t>Own Use</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Bhuvan Testing</t>
   </si>
 </sst>
 </file>
@@ -682,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>8</v>
@@ -703,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>25</v>
@@ -742,7 +757,7 @@
         <v>38</v>
       </c>
       <c r="X3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.4">
@@ -793,16 +808,16 @@
         <v>34</v>
       </c>
       <c r="U4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="W4" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.4">
@@ -816,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
@@ -834,15 +849,27 @@
         <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>23</v>
       </c>
@@ -853,16 +880,16 @@
         <v>34</v>
       </c>
       <c r="U5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="W5" s="7">
         <v>6</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -875,7 +902,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{147F5B5B-A653-4F7A-9371-88FE8BC0D8D7}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{7EF10CD1-CDB9-4436-B4A4-9886E081532C}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{21442B46-9264-4E3A-AB7F-FEC50167BF58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>